<commit_message>
sobre 20 -> 25
</commit_message>
<xml_diff>
--- a/tabela.xlsx
+++ b/tabela.xlsx
@@ -524,7 +524,7 @@
   <dimension ref="B2:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,7 +609,7 @@
         <v>9</v>
       </c>
       <c r="C12" s="9">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">

</xml_diff>